<commit_message>
Fix Streamlit file uploader API exception using dynamic key; misc updates
</commit_message>
<xml_diff>
--- a/Vendor_branch.xlsx
+++ b/Vendor_branch.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\ocr\AppViewCPFS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\ocr\view_ocr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E036776A-0D5D-4BFF-9219-B72FF035CEFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BA5437B-C5DC-4F76-BC18-A4F602D85F9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3765" yWindow="2520" windowWidth="21600" windowHeight="11235" xr2:uid="{6506BE60-3C73-4701-8988-81E5CDE8235E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6506BE60-3C73-4701-8988-81E5CDE8235E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -476,10 +476,10 @@
     <t>0107542000011</t>
   </si>
   <si>
+    <t>ALL00001</t>
+  </si>
+  <si>
     <t>บริษัท ซีพี ออลล์ จำกัด (มหาชน)</t>
-  </si>
-  <si>
-    <t>ALL00001</t>
   </si>
 </sst>
 </file>
@@ -1072,8 +1072,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11ACC454-015B-4582-9B54-6E306FF53C87}">
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="E50" sqref="E50"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1906,7 +1906,7 @@
         <v>145</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C49" s="11" t="s">
         <v>97</v>
@@ -1915,7 +1915,7 @@
         <v>5</v>
       </c>
       <c r="E49" s="14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -1927,26 +1927,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="9ea82972-d7d5-4eaf-919e-93bb6e68076d" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0cd7e064-e400-4284-9400-fb553c28cffa">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000415EE01BF4D804280F380F9DB1CFF0D" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3a0889e59f2beebff0116b3924e2bba8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0cd7e064-e400-4284-9400-fb553c28cffa" xmlns:ns3="9ea82972-d7d5-4eaf-919e-93bb6e68076d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a759d0038229a5f52eef73949470c7e5" ns2:_="" ns3:_="">
     <xsd:import namespace="0cd7e064-e400-4284-9400-fb553c28cffa"/>
@@ -2141,10 +2121,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="9ea82972-d7d5-4eaf-919e-93bb6e68076d" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0cd7e064-e400-4284-9400-fb553c28cffa">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1C2E36A-EC7F-423F-8D14-19D21DB059CD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{25A85255-B37F-41AE-9392-794E41C222F1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="0cd7e064-e400-4284-9400-fb553c28cffa"/>
+    <ds:schemaRef ds:uri="9ea82972-d7d5-4eaf-919e-93bb6e68076d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2161,20 +2172,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{25A85255-B37F-41AE-9392-794E41C222F1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1C2E36A-EC7F-423F-8D14-19D21DB059CD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="0cd7e064-e400-4284-9400-fb553c28cffa"/>
-    <ds:schemaRef ds:uri="9ea82972-d7d5-4eaf-919e-93bb6e68076d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>